<commit_message>
plotted sonication temp profile for metallic inks
</commit_message>
<xml_diff>
--- a/data_plotting/temp_sonicate/Ag_EMD5800_ice_9_15_16.xlsx
+++ b/data_plotting/temp_sonicate/Ag_EMD5800_ice_9_15_16.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\Michael Orrill\Documents\local_repo\data_plotting\temp_sonicate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="360" windowWidth="17955" windowHeight="11535"/>
   </bookViews>
@@ -3762,7 +3767,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3803,6 +3808,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3851,7 +3859,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3884,9 +3892,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3919,6 +3944,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">

</xml_diff>